<commit_message>
Se sube version presentada al profe
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\PROYECTO DE GRADO\PROYECTO ANYLOGIC\Modelo-simulacion-delitos-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hewlett Packard\Desktop\Nueva carpeta\Modelo-simulacion-delitos-\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893A5D93-69D3-417F-B1AA-CB620C28DBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19185" windowHeight="6615" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="CAI" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="33">
   <si>
     <t>Location</t>
   </si>
@@ -129,7 +130,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -187,14 +188,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -479,7 +476,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -507,10 +504,10 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3">
+      <c r="B2" s="2">
         <v>71539</v>
       </c>
-      <c r="C2" s="4">
+      <c r="C2">
         <v>-73.133399999999995</v>
       </c>
     </row>
@@ -518,10 +515,10 @@
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="3">
+      <c r="B3" s="2">
         <v>71229</v>
       </c>
-      <c r="C3" s="4">
+      <c r="C3">
         <v>-73.122100000000003</v>
       </c>
     </row>
@@ -529,10 +526,10 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="3">
+      <c r="B4" s="2">
         <v>71237</v>
       </c>
-      <c r="C4" s="4">
+      <c r="C4">
         <v>-73133</v>
       </c>
     </row>
@@ -540,10 +537,10 @@
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="3">
+      <c r="B5" s="2">
         <v>71415</v>
       </c>
-      <c r="C5" s="4">
+      <c r="C5">
         <v>-73.132900000000006</v>
       </c>
     </row>
@@ -551,10 +548,10 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="3">
+      <c r="B6" s="2">
         <v>71225</v>
       </c>
-      <c r="C6" s="4">
+      <c r="C6">
         <v>-73.125200000000007</v>
       </c>
     </row>
@@ -562,10 +559,10 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="3">
+      <c r="B7" s="2">
         <v>71194</v>
       </c>
-      <c r="C7" s="4">
+      <c r="C7">
         <v>-73.109200000000001</v>
       </c>
     </row>
@@ -573,10 +570,10 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="3">
+      <c r="B8" s="2">
         <v>70972</v>
       </c>
-      <c r="C8" s="4">
+      <c r="C8">
         <v>-73.110399999999998</v>
       </c>
     </row>
@@ -584,10 +581,10 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="3">
+      <c r="B9" s="2">
         <v>71132</v>
       </c>
-      <c r="C9" s="4">
+      <c r="C9">
         <v>-73.106399999999994</v>
       </c>
     </row>
@@ -595,10 +592,10 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="3">
+      <c r="B10" s="2">
         <v>71169</v>
       </c>
-      <c r="C10" s="4">
+      <c r="C10">
         <v>-73.112300000000005</v>
       </c>
     </row>
@@ -606,10 +603,10 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="3">
+      <c r="B11" s="2">
         <v>70858</v>
       </c>
-      <c r="C11" s="4">
+      <c r="C11">
         <v>-73.117000000000004</v>
       </c>
     </row>
@@ -617,10 +614,10 @@
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="2">
         <v>71279</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12">
         <v>-73.109700000000004</v>
       </c>
     </row>
@@ -628,10 +625,10 @@
       <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="2">
         <v>71324</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13">
         <v>-73.112799999999993</v>
       </c>
     </row>
@@ -642,11 +639,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F16"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -669,10 +666,10 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2" s="2">
+      <c r="B2">
         <v>7.1513499999999999</v>
       </c>
-      <c r="C2" s="2">
+      <c r="C2">
         <v>-73.144999999999996</v>
       </c>
     </row>
@@ -680,10 +677,10 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2">
+      <c r="B3">
         <v>7.12</v>
       </c>
-      <c r="C3" s="2">
+      <c r="C3">
         <v>-73.116</v>
       </c>
     </row>
@@ -691,10 +688,10 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="2">
+      <c r="B4">
         <v>7.1705500000000004</v>
       </c>
-      <c r="C4" s="2">
+      <c r="C4">
         <v>-73.135000000000005</v>
       </c>
     </row>
@@ -702,10 +699,10 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5" s="2">
+      <c r="B5">
         <v>7.18668</v>
       </c>
-      <c r="C5" s="2">
+      <c r="C5">
         <v>-73.130298999999994</v>
       </c>
     </row>
@@ -713,10 +710,10 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2">
+      <c r="B6">
         <v>7.1780400000000002</v>
       </c>
-      <c r="C6" s="2">
+      <c r="C6">
         <v>-73.130223999999998</v>
       </c>
     </row>
@@ -724,10 +721,10 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="2">
+      <c r="B7">
         <v>7.1163299999999996</v>
       </c>
-      <c r="C7" s="2">
+      <c r="C7">
         <v>-73.129890000000003</v>
       </c>
     </row>
@@ -735,101 +732,266 @@
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="2">
+      <c r="B8">
         <v>7.1159999999999997</v>
       </c>
-      <c r="C8" s="2">
+      <c r="C8">
         <v>-73.126999999999995</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9" s="2">
+      <c r="B9">
         <v>7.091882</v>
       </c>
-      <c r="C9" s="2">
+      <c r="C9">
         <v>-73.109082000000001</v>
       </c>
-      <c r="E9" s="7"/>
+      <c r="E9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="5">
+      <c r="B10" s="2">
         <v>7117348</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10">
         <v>-73.129052999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="8" t="s">
+      <c r="A11" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="5">
+      <c r="B11" s="2">
         <v>7118031</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11">
         <v>-73.117840999999999</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="5">
+      <c r="B12" s="2">
         <v>7125948</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12">
         <v>-73.113600000000005</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="5">
+      <c r="B13" s="2">
         <v>7128164</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13">
         <v>-73.130927999999997</v>
       </c>
-      <c r="F13" s="7"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="9" t="s">
+      <c r="A14" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="5">
+      <c r="B14" s="2">
         <v>714255</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14">
         <v>-73.120199999999997</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="8" t="s">
+      <c r="A15" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="5">
+      <c r="B15" s="2">
         <v>7149916</v>
       </c>
-      <c r="C15" s="6">
+      <c r="C15">
         <v>-73.135418999999999</v>
       </c>
-      <c r="F15" s="7"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="5">
+      <c r="B16" s="2">
         <v>7133093</v>
       </c>
-      <c r="C16" s="6">
+      <c r="C16">
+        <v>-73.115200000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>9</v>
+      </c>
+      <c r="B17">
+        <v>7.1513499999999999</v>
+      </c>
+      <c r="C17">
+        <v>-73.144999999999996</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18">
+        <v>7.12</v>
+      </c>
+      <c r="C18">
+        <v>-73.116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>11</v>
+      </c>
+      <c r="B19">
+        <v>7.1705500000000004</v>
+      </c>
+      <c r="C19">
+        <v>-73.135000000000005</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>12</v>
+      </c>
+      <c r="B20">
+        <v>7.18668</v>
+      </c>
+      <c r="C20">
+        <v>-73.130298999999994</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21">
+        <v>7.1780400000000002</v>
+      </c>
+      <c r="C21">
+        <v>-73.130223999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22">
+        <v>7.1163299999999996</v>
+      </c>
+      <c r="C22">
+        <v>-73.129890000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>16</v>
+      </c>
+      <c r="B23">
+        <v>7.1159999999999997</v>
+      </c>
+      <c r="C23">
+        <v>-73.126999999999995</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24">
+        <v>7.091882</v>
+      </c>
+      <c r="C24">
+        <v>-73.109082000000001</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B25" s="2">
+        <v>7117348</v>
+      </c>
+      <c r="C25">
+        <v>-73.129052999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B26" s="2">
+        <v>7118031</v>
+      </c>
+      <c r="C26">
+        <v>-73.117840999999999</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2">
+        <v>7125948</v>
+      </c>
+      <c r="C27">
+        <v>-73.113600000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>29</v>
+      </c>
+      <c r="B28" s="2">
+        <v>7128164</v>
+      </c>
+      <c r="C28">
+        <v>-73.130927999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B29" s="2">
+        <v>714255</v>
+      </c>
+      <c r="C29">
+        <v>-73.120199999999997</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B30" s="2">
+        <v>7149916</v>
+      </c>
+      <c r="C30">
+        <v>-73.135418999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2">
+        <v>7133093</v>
+      </c>
+      <c r="C31">
         <v>-73.115200000000002</v>
       </c>
     </row>

</xml_diff>

<commit_message>
actualizacion datos en DATA
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hewlett Packard\Desktop\Nueva carpeta\Modelo-simulacion-delitos-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Usuario\Desktop\PROYECTO DE GRADO\PROYECTO ANYLOGIC\Modelo-simulacion-delitos-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{893A5D93-69D3-417F-B1AA-CB620C28DBE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20640" windowHeight="11160" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="CAI" sheetId="1" r:id="rId1"/>
@@ -130,7 +129,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -191,12 +190,12 @@
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,11 +475,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E12" sqref="E12"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -504,8 +503,8 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="2">
-        <v>71539</v>
+      <c r="B2" s="5">
+        <v>7.1539000000000001</v>
       </c>
       <c r="C2">
         <v>-73.133399999999995</v>
@@ -515,8 +514,8 @@
       <c r="A3" t="s">
         <v>22</v>
       </c>
-      <c r="B3" s="2">
-        <v>71229</v>
+      <c r="B3" s="5">
+        <v>7.1228999999999996</v>
       </c>
       <c r="C3">
         <v>-73.122100000000003</v>
@@ -526,19 +525,19 @@
       <c r="A4" t="s">
         <v>23</v>
       </c>
-      <c r="B4" s="2">
-        <v>71237</v>
+      <c r="B4" s="5">
+        <v>7.1237000000000004</v>
       </c>
       <c r="C4">
-        <v>-73133</v>
+        <v>-73.132999999999996</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>15</v>
       </c>
-      <c r="B5" s="2">
-        <v>71415</v>
+      <c r="B5" s="5">
+        <v>7.1414999999999997</v>
       </c>
       <c r="C5">
         <v>-73.132900000000006</v>
@@ -548,8 +547,8 @@
       <c r="A6" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2">
-        <v>71225</v>
+      <c r="B6" s="5">
+        <v>7.1224999999999996</v>
       </c>
       <c r="C6">
         <v>-73.125200000000007</v>
@@ -559,8 +558,8 @@
       <c r="A7" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2">
-        <v>71194</v>
+      <c r="B7" s="5">
+        <v>7.1193999999999997</v>
       </c>
       <c r="C7">
         <v>-73.109200000000001</v>
@@ -570,8 +569,8 @@
       <c r="A8" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="2">
-        <v>70972</v>
+      <c r="B8" s="5">
+        <v>7.0972</v>
       </c>
       <c r="C8">
         <v>-73.110399999999998</v>
@@ -581,8 +580,8 @@
       <c r="A9" t="s">
         <v>5</v>
       </c>
-      <c r="B9" s="2">
-        <v>71132</v>
+      <c r="B9" s="5">
+        <v>7.1132</v>
       </c>
       <c r="C9">
         <v>-73.106399999999994</v>
@@ -592,8 +591,8 @@
       <c r="A10" t="s">
         <v>6</v>
       </c>
-      <c r="B10" s="2">
-        <v>71169</v>
+      <c r="B10" s="5">
+        <v>7.1169000000000002</v>
       </c>
       <c r="C10">
         <v>-73.112300000000005</v>
@@ -603,8 +602,8 @@
       <c r="A11" t="s">
         <v>7</v>
       </c>
-      <c r="B11" s="2">
-        <v>70858</v>
+      <c r="B11" s="5">
+        <v>7.0857999999999999</v>
       </c>
       <c r="C11">
         <v>-73.117000000000004</v>
@@ -614,8 +613,8 @@
       <c r="A12" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="2">
-        <v>71279</v>
+      <c r="B12" s="5">
+        <v>7.1279000000000003</v>
       </c>
       <c r="C12">
         <v>-73.109700000000004</v>
@@ -625,8 +624,8 @@
       <c r="A13" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="2">
-        <v>71324</v>
+      <c r="B13" s="5">
+        <v>7.1323999999999996</v>
       </c>
       <c r="C13">
         <v>-73.112799999999993</v>
@@ -639,11 +638,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,7 +665,7 @@
       <c r="A2" t="s">
         <v>9</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="5">
         <v>7.1513499999999999</v>
       </c>
       <c r="C2">
@@ -677,7 +676,7 @@
       <c r="A3" t="s">
         <v>10</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="5">
         <v>7.12</v>
       </c>
       <c r="C3">
@@ -688,7 +687,7 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="5">
         <v>7.1705500000000004</v>
       </c>
       <c r="C4">
@@ -699,7 +698,7 @@
       <c r="A5" t="s">
         <v>12</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="5">
         <v>7.18668</v>
       </c>
       <c r="C5">
@@ -710,7 +709,7 @@
       <c r="A6" t="s">
         <v>13</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="5">
         <v>7.1780400000000002</v>
       </c>
       <c r="C6">
@@ -721,7 +720,7 @@
       <c r="A7" t="s">
         <v>14</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="5">
         <v>7.1163299999999996</v>
       </c>
       <c r="C7">
@@ -732,7 +731,7 @@
       <c r="A8" t="s">
         <v>16</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="5">
         <v>7.1159999999999997</v>
       </c>
       <c r="C8">
@@ -743,31 +742,31 @@
       <c r="A9" t="s">
         <v>19</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>7.091882</v>
       </c>
       <c r="C9">
         <v>-73.109082000000001</v>
       </c>
-      <c r="E9" s="3"/>
+      <c r="E9" s="2"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>26</v>
       </c>
-      <c r="B10" s="2">
-        <v>7117348</v>
+      <c r="B10" s="5">
+        <v>7.1173479999999998</v>
       </c>
       <c r="C10">
         <v>-73.129052999999999</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="4" t="s">
+      <c r="A11" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B11" s="2">
-        <v>7118031</v>
+      <c r="B11" s="5">
+        <v>7.1180310000000002</v>
       </c>
       <c r="C11">
         <v>-73.117840999999999</v>
@@ -777,8 +776,8 @@
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="2">
-        <v>7125948</v>
+      <c r="B12" s="5">
+        <v>7.1259480000000002</v>
       </c>
       <c r="C12">
         <v>-73.113600000000005</v>
@@ -788,43 +787,43 @@
       <c r="A13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="2">
-        <v>7128164</v>
+      <c r="B13" s="5">
+        <v>7.1281639999999999</v>
       </c>
       <c r="C13">
         <v>-73.130927999999997</v>
       </c>
-      <c r="F13" s="3"/>
+      <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B14" s="2">
-        <v>714255</v>
+      <c r="B14" s="5">
+        <v>7.14255</v>
       </c>
       <c r="C14">
         <v>-73.120199999999997</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B15" s="2">
-        <v>7149916</v>
+      <c r="B15" s="5">
+        <v>7.1499160000000002</v>
       </c>
       <c r="C15">
         <v>-73.135418999999999</v>
       </c>
-      <c r="F15" s="3"/>
+      <c r="F15" s="2"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="4" t="s">
+      <c r="A16" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="2">
-        <v>7133093</v>
+      <c r="B16" s="5">
+        <v>7.1330929999999997</v>
       </c>
       <c r="C16">
         <v>-73.115200000000002</v>
@@ -834,7 +833,7 @@
       <c r="A17" t="s">
         <v>9</v>
       </c>
-      <c r="B17">
+      <c r="B17" s="5">
         <v>7.1513499999999999</v>
       </c>
       <c r="C17">
@@ -845,7 +844,7 @@
       <c r="A18" t="s">
         <v>10</v>
       </c>
-      <c r="B18">
+      <c r="B18" s="5">
         <v>7.12</v>
       </c>
       <c r="C18">
@@ -856,7 +855,7 @@
       <c r="A19" t="s">
         <v>11</v>
       </c>
-      <c r="B19">
+      <c r="B19" s="5">
         <v>7.1705500000000004</v>
       </c>
       <c r="C19">
@@ -867,7 +866,7 @@
       <c r="A20" t="s">
         <v>12</v>
       </c>
-      <c r="B20">
+      <c r="B20" s="5">
         <v>7.18668</v>
       </c>
       <c r="C20">
@@ -878,7 +877,7 @@
       <c r="A21" t="s">
         <v>13</v>
       </c>
-      <c r="B21">
+      <c r="B21" s="5">
         <v>7.1780400000000002</v>
       </c>
       <c r="C21">
@@ -889,7 +888,7 @@
       <c r="A22" t="s">
         <v>14</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <v>7.1163299999999996</v>
       </c>
       <c r="C22">
@@ -900,7 +899,7 @@
       <c r="A23" t="s">
         <v>16</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>7.1159999999999997</v>
       </c>
       <c r="C23">
@@ -911,7 +910,7 @@
       <c r="A24" t="s">
         <v>19</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <v>7.091882</v>
       </c>
       <c r="C24">
@@ -922,19 +921,19 @@
       <c r="A25" t="s">
         <v>26</v>
       </c>
-      <c r="B25" s="2">
-        <v>7117348</v>
+      <c r="B25" s="5">
+        <v>7.1173479999999998</v>
       </c>
       <c r="C25">
         <v>-73.129052999999999</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="4" t="s">
+      <c r="A26" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B26" s="2">
-        <v>7118031</v>
+      <c r="B26" s="5">
+        <v>7.1180310000000002</v>
       </c>
       <c r="C26">
         <v>-73.117840999999999</v>
@@ -944,8 +943,8 @@
       <c r="A27" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2">
-        <v>7125948</v>
+      <c r="B27" s="5">
+        <v>7.1259480000000002</v>
       </c>
       <c r="C27">
         <v>-73.113600000000005</v>
@@ -955,41 +954,41 @@
       <c r="A28" t="s">
         <v>29</v>
       </c>
-      <c r="B28" s="2">
-        <v>7128164</v>
+      <c r="B28" s="5">
+        <v>7.1281639999999999</v>
       </c>
       <c r="C28">
         <v>-73.130927999999997</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="5" t="s">
+      <c r="A29" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="2">
-        <v>714255</v>
+      <c r="B29" s="5">
+        <v>7.14255</v>
       </c>
       <c r="C29">
         <v>-73.120199999999997</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="4" t="s">
+      <c r="A30" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2">
-        <v>7149916</v>
+      <c r="B30" s="5">
+        <v>7.1499160000000002</v>
       </c>
       <c r="C30">
         <v>-73.135418999999999</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="4" t="s">
+      <c r="A31" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B31" s="2">
-        <v>7133093</v>
+      <c r="B31" s="5">
+        <v>7.1330929999999997</v>
       </c>
       <c r="C31">
         <v>-73.115200000000002</v>

</xml_diff>

<commit_message>
hay ERROR en validar llegada otras patrullas
</commit_message>
<xml_diff>
--- a/DATA.xlsx
+++ b/DATA.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="139">
   <si>
     <t>CAI Kennedy</t>
   </si>
@@ -436,13 +436,19 @@
   </si>
   <si>
     <t>creado</t>
+  </si>
+  <si>
+    <t>id_delito</t>
+  </si>
+  <si>
+    <t>id_cai</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -457,13 +463,6 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="9"/>
-      <color rgb="FF1A73E8"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -510,14 +509,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="22" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -798,213 +797,255 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F14"/>
+  <dimension ref="A1:G14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31" customWidth="1"/>
-    <col min="2" max="2" width="34.7109375" customWidth="1"/>
-    <col min="3" max="3" width="31.140625" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" customWidth="1"/>
+    <col min="2" max="2" width="31" customWidth="1"/>
+    <col min="3" max="3" width="34.7109375" customWidth="1"/>
+    <col min="4" max="4" width="31.140625" customWidth="1"/>
+    <col min="6" max="6" width="35.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2" s="8" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="7" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>74</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="F3" t="s">
+      <c r="G3" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>79</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>80</v>
       </c>
-      <c r="E5" t="s">
-        <v>26</v>
-      </c>
       <c r="F5" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="G5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>82</v>
       </c>
-      <c r="E6" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="E7" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="E8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>4</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="E9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>5</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="F10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+      <c r="G10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>16</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="E12" t="s">
+      <c r="F12" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>17</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="E13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="F13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>70</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="F14" t="s">
+      <c r="G14" t="s">
         <v>72</v>
       </c>
     </row>
@@ -1016,492 +1057,655 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G31"/>
+  <dimension ref="A1:H31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="44.85546875" customWidth="1"/>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="16.28515625" customWidth="1"/>
-    <col min="4" max="4" width="37.140625" customWidth="1"/>
-    <col min="6" max="6" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="44.85546875" customWidth="1"/>
+    <col min="3" max="3" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="16.28515625" customWidth="1"/>
+    <col min="5" max="5" width="37.140625" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="7">
+      <c r="E2" s="6">
         <v>45440.492708333331</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="F2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="D3" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="7">
+      <c r="E3" s="6">
         <v>45414.365891203706</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="F3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="D4" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D4" s="7">
+      <c r="E4" s="6">
         <v>45445.853263888886</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
+      <c r="F4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>23</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="C5" s="5" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E5" s="6">
         <v>45591.329085648147</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
+      <c r="F5" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="C6" s="5" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="6" t="s">
+      <c r="D6" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="6">
         <v>45351.534479166665</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
+      <c r="F6" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
         <v>24</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="D7" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="6">
         <v>45674.351273148146</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
+      <c r="F7" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
         <v>11</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="C8" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E8" s="6">
         <v>45519.15353009259</v>
       </c>
-      <c r="G8" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
+      <c r="F8" s="8">
+        <v>0</v>
+      </c>
+      <c r="H8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="D9" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E9" s="6">
         <v>45487.360937500001</v>
       </c>
-      <c r="G9" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+      <c r="F9" s="8">
+        <v>0</v>
+      </c>
+      <c r="H9" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="D10" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="D10" s="7">
+      <c r="E10" s="6">
         <v>45562.531770833331</v>
       </c>
-      <c r="G10" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="8">
+        <v>0</v>
+      </c>
+      <c r="H10" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="D11" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E11" s="6">
         <v>45329.573981481481</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="F11" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>28</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="D12" s="5" t="s">
         <v>57</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E12" s="6">
         <v>45329.573981481481</v>
       </c>
-      <c r="F12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="F12" s="8">
+        <v>0</v>
+      </c>
+      <c r="G12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>29</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="D13" s="5" t="s">
         <v>58</v>
       </c>
-      <c r="D13" s="7">
+      <c r="E13" s="6">
         <v>45342.275208333333</v>
       </c>
-      <c r="E13" s="2"/>
-      <c r="F13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A14" s="4" t="s">
+      <c r="F13" s="8">
+        <v>0</v>
+      </c>
+      <c r="G13" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B14" s="6" t="s">
+      <c r="C14" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C14" s="6" t="s">
+      <c r="D14" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="D14" s="7">
+      <c r="E14" s="6">
         <v>45402.928287037037</v>
       </c>
-      <c r="F14" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="F14" s="8">
+        <v>0</v>
+      </c>
+      <c r="G14" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="D15" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="D15" s="7">
+      <c r="E15" s="6">
         <v>45524.678518518522</v>
       </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="5"/>
-    </row>
-    <row r="16" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
+      <c r="F15" s="8">
+        <v>0</v>
+      </c>
+      <c r="G15" s="4"/>
+    </row>
+    <row r="16" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="D16" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="D16" s="7">
+      <c r="E16" s="6">
         <v>45546.539756944447</v>
       </c>
-      <c r="F16" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="F16" s="8">
+        <v>0</v>
+      </c>
+      <c r="G16" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="6" t="s">
+      <c r="C17" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C17" s="6" t="s">
+      <c r="D17" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="D17" s="7">
+      <c r="E17" s="6">
         <v>45459.615127314813</v>
       </c>
-      <c r="F17" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="F17" s="8">
+        <v>0</v>
+      </c>
+      <c r="G17" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>30</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="D18" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D18" s="7">
+      <c r="E18" s="6">
         <v>45535.895972222221</v>
       </c>
-      <c r="F18" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+      <c r="F18" s="8">
+        <v>0</v>
+      </c>
+      <c r="G18" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>31</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="D19" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D19" s="7">
+      <c r="E19" s="6">
         <v>45546.648842592593</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F19" s="8">
+        <v>0</v>
+      </c>
+      <c r="G19" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="20" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>32</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="D20" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="D20" s="7">
+      <c r="E20" s="6">
         <v>45387.779409722221</v>
       </c>
-      <c r="F20" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="F20" s="8">
+        <v>0</v>
+      </c>
+      <c r="G20" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="D21" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="D21" s="7">
+      <c r="E21" s="6">
         <v>45512.785740740743</v>
       </c>
-      <c r="F21" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+      <c r="F21" s="8">
+        <v>0</v>
+      </c>
+      <c r="G21" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>34</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="D22" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="F22" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
+      <c r="F22" s="8">
+        <v>0</v>
+      </c>
+      <c r="G22" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
         <v>59</v>
       </c>
-      <c r="B23" s="6" t="s">
+      <c r="C23" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C23" s="6" t="s">
+      <c r="D23" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="F23" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="F23" s="8">
+        <v>0</v>
+      </c>
+      <c r="G23" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
         <v>61</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="D24" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="F24" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
+      <c r="F24" s="8">
+        <v>0</v>
+      </c>
+      <c r="G24" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
         <v>62</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="D25" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="E25" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+      <c r="F25" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
         <v>63</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="D26" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="E26" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="F26" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>64</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="D27" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="E27" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+      <c r="F27" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>65</v>
       </c>
-      <c r="B28" s="6" t="s">
+      <c r="C28" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C28" s="6" t="s">
+      <c r="D28" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="E28" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="F28" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="D29" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="E29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A30" s="3" t="s">
+      <c r="F29" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="2" t="s">
         <v>67</v>
       </c>
-      <c r="B30" s="6" t="s">
+      <c r="C30" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C30" s="6" t="s">
+      <c r="D30" s="5" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A31" s="3" t="s">
+      <c r="F30" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="D31" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="E31" t="s">
-        <v>26</v>
+      <c r="F31" s="8">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>